<commit_message>
refactor: update configuration settings in config.py; enhance user input prompts in DataEngineer agent; improve message handling in DataTeamManager agent; add data profiling functionality in DataQualityAnalyst agent; streamline utility functions for better code organization
</commit_message>
<xml_diff>
--- a/data_to_model.xlsx
+++ b/data_to_model.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nigam\Documents\AutoMMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516B4E44-821B-419F-9632-5D09F176C05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5D60E5-1D27-45A9-B9DE-8661A3F32D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6825" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10272" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="22">
   <si>
     <t>branded_spends</t>
   </si>
@@ -13297,8 +13298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="F269" sqref="F269"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -27910,4 +27911,98 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A81EB0-1C8E-4FC3-97F3-226EEA4DA6BC}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="31.20703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1015625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>